<commit_message>
docs:  update to test report
</commit_message>
<xml_diff>
--- a/Test Report.xlsx
+++ b/Test Report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t xml:space="preserve">Scenario ID </t>
   </si>
@@ -146,13 +146,22 @@
   </si>
   <si>
     <t>User should be able to see his order after successful checkout under my orders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL SCENARIOS EXECUTED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASSED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAILED </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -175,8 +184,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF38761D"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +208,12 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1C232"/>
+        <bgColor rgb="FFF1C232"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -196,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -236,6 +261,18 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,15 +743,30 @@
       <c r="D20" s="13"/>
     </row>
     <row r="21">
-      <c r="B21" s="12"/>
+      <c r="B21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="15">
+        <v>17.0</v>
+      </c>
       <c r="D21" s="13"/>
     </row>
     <row r="22">
-      <c r="B22" s="12"/>
+      <c r="B22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="16">
+        <v>16.0</v>
+      </c>
       <c r="D22" s="13"/>
     </row>
     <row r="23">
-      <c r="B23" s="12"/>
+      <c r="B23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="17">
+        <v>1.0</v>
+      </c>
       <c r="D23" s="13"/>
     </row>
     <row r="24">
@@ -4615,9 +4667,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C12"/>
     <mergeCell ref="C13:C18"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D997">

</xml_diff>